<commit_message>
formatted testplanresults and added an installation guide
</commit_message>
<xml_diff>
--- a/LastPresentation/TrackModel/testplanresults.xlsx
+++ b/LastPresentation/TrackModel/testplanresults.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Testing Steps</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>repeat step 6 except now is closed should say false</t>
+  </si>
+  <si>
+    <t>Track Model Test Plan Results</t>
+  </si>
+  <si>
+    <t>Author: Sarah Bunke</t>
+  </si>
+  <si>
+    <t>Tester: Saraah Bunke</t>
   </si>
 </sst>
 </file>
@@ -114,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -122,15 +131,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,158 +512,267 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="7" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E12" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="13" spans="1:5" s="1" customFormat="1" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B21" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D21" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E21" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="22" spans="1:5" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+    </row>
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>24</v>
       </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>